<commit_message>
pivot: improve format matching, add empty cell checking to tests
The patch improves the pivot table cell format matching with the
output data, so we check if there is a complete match or a partial
match. A partial match is when we found one match for a field, but
other fields are not set, and if this partial match is found in
exactly 1 line of output data, then we treat it as a complete match.

This also refactors the code so there is code no duplication for
column and row matching code - they work in the same way, just
in a different orientation.

This also adds checking of empty cells to the tests, so we can
make sure there is no other cell in the pivot table that got the
pivot table cell format applied to. A new test case was also added
to the test class.

Change-Id: I102ec8e33bc7a3f26bc898568ee0e33abe08bd27
Reviewed-on: https://gerrit.libreoffice.org/c/core/+/166086
Tested-by: Tomaž Vajngerl <quikee@gmail.com>
Reviewed-by: Tomaž Vajngerl <quikee@gmail.com>
</commit_message>
<xml_diff>
--- a/sc/qa/unit/data/xlsx/pivot-table/PivotTableCellFormatsTest_2_DataFieldInRow_ColumnLabelColor.xlsx
+++ b/sc/qa/unit/data/xlsx/pivot-table/PivotTableCellFormatsTest_2_DataFieldInRow_ColumnLabelColor.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\VBOXSVR\quikee\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B861FA5-F8E0-42B0-9E5B-20AC1B24358A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE39009C-A295-49D8-B2D8-CA836453FF3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="27288" windowHeight="16224" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,37 +40,22 @@
     <t>Sum of C</t>
   </si>
   <si>
-    <t>Values</t>
+    <t>Sum of D</t>
   </si>
   <si>
-    <t>Sum of D</t>
+    <t>Values</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF00B0F0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -119,6 +104,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF999999"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="65"/>
       </left>
@@ -141,17 +137,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF999999"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF999999"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF999999"/>
       </left>
@@ -188,7 +173,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -198,49 +183,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" pivotButton="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" pivotButton="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <b/>
-        <family val="2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -259,72 +242,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3CF43B21-4365-AD79-48AA-2D64711B9B93}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="3611880" y="1645920"/>
-          <a:ext cx="3238500" cy="739140"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -401,27 +318,25 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="0" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" showDrill="0" colGrandTotals="0" createdVersion="8" indent="0" compact="0" outline="1" compactData="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="0" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" showDrill="0" rowGrandTotals="0" colGrandTotals="0" createdVersion="8" indent="0" compact="0" outline="1" compactData="0">
   <location ref="G4:K7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
-    <pivotField axis="axisCol" compact="0" showAll="0">
-      <items count="5">
+    <pivotField axis="axisCol" compact="0" showAll="0" defaultSubtotal="0">
+      <items count="4">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
         <item x="3"/>
-        <item t="default"/>
       </items>
     </pivotField>
-    <pivotField compact="0" showAll="0">
-      <items count="3">
+    <pivotField compact="0" showAll="0" defaultSubtotal="0">
+      <items count="2">
         <item x="0"/>
         <item x="1"/>
-        <item t="default"/>
       </items>
     </pivotField>
-    <pivotField dataField="1" compact="0" showAll="0"/>
-    <pivotField dataField="1" compact="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" compact="0" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
   <rowFields count="1">
     <field x="-2"/>
@@ -455,36 +370,12 @@
     <dataField name="Sum of C" fld="2" baseField="0" baseItem="0"/>
     <dataField name="Sum of D" fld="3" baseField="0" baseItem="0"/>
   </dataFields>
-  <formats count="3">
-    <format dxfId="2">
+  <formats count="1">
+    <format dxfId="0">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
             <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="1">
-      <pivotArea outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="0">
-      <pivotArea outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="1"/>
           </reference>
         </references>
       </pivotArea>
@@ -496,7 +387,7 @@
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
     </ext>
     <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
     </ext>
   </extLst>
 </pivotTableDefinition>
@@ -763,7 +654,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -836,12 +727,12 @@
         <v>6</v>
       </c>
       <c r="G4" s="1"/>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
-      <c r="K4" s="3"/>
+      <c r="K4" s="5"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5">
@@ -856,19 +747,19 @@
       <c r="D5">
         <v>10</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" s="9">
+      <c r="G5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="14">
         <v>1</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="6">
         <v>2</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="6">
         <v>3</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="4">
         <v>4</v>
       </c>
     </row>
@@ -876,38 +767,37 @@
       <c r="G6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="7">
         <v>3</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="8">
         <v>3</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6" s="8">
         <v>4</v>
       </c>
-      <c r="K6" s="6">
+      <c r="K6" s="9">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:11">
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" s="11">
+        <v>7</v>
+      </c>
+      <c r="I7" s="12">
+        <v>2</v>
+      </c>
+      <c r="J7" s="12">
         <v>6</v>
       </c>
-      <c r="H7" s="7">
-        <v>7</v>
-      </c>
-      <c r="I7" s="8">
-        <v>2</v>
-      </c>
-      <c r="J7" s="8">
-        <v>6</v>
-      </c>
-      <c r="K7" s="10">
+      <c r="K7" s="13">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>